<commit_message>
added some more data, stuff is still running ..
</commit_message>
<xml_diff>
--- a/M0.2D0.0001E0.9A0.8_100x100_MC25_table_experiment.xlsx
+++ b/M0.2D0.0001E0.9A0.8_100x100_MC25_table_experiment.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G104"/>
+  <dimension ref="A1:G136"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3045,6 +3045,806 @@
         <v>0.8008999999999999</v>
       </c>
     </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B105" t="n">
+        <v>774999</v>
+      </c>
+      <c r="C105" t="n">
+        <v>1</v>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>[1596]</t>
+        </is>
+      </c>
+      <c r="E105" t="n">
+        <v>1596</v>
+      </c>
+      <c r="F105" t="n">
+        <v>2003</v>
+      </c>
+      <c r="G105" t="n">
+        <v>0.7968</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B106" t="n">
+        <v>349999</v>
+      </c>
+      <c r="C106" t="n">
+        <v>1</v>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>[1644]</t>
+        </is>
+      </c>
+      <c r="E106" t="n">
+        <v>1644</v>
+      </c>
+      <c r="F106" t="n">
+        <v>2044</v>
+      </c>
+      <c r="G106" t="n">
+        <v>0.8043</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B107" t="n">
+        <v>1074999</v>
+      </c>
+      <c r="C107" t="n">
+        <v>1</v>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>[1581]</t>
+        </is>
+      </c>
+      <c r="E107" t="n">
+        <v>1581</v>
+      </c>
+      <c r="F107" t="n">
+        <v>1989</v>
+      </c>
+      <c r="G107" t="n">
+        <v>0.7949000000000001</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>2028</v>
+      </c>
+      <c r="B108" t="n">
+        <v>274999</v>
+      </c>
+      <c r="C108" t="n">
+        <v>1</v>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>[1583]</t>
+        </is>
+      </c>
+      <c r="E108" t="n">
+        <v>1583</v>
+      </c>
+      <c r="F108" t="n">
+        <v>1993</v>
+      </c>
+      <c r="G108" t="n">
+        <v>0.7943</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>2032</v>
+      </c>
+      <c r="B109" t="n">
+        <v>574999</v>
+      </c>
+      <c r="C109" t="n">
+        <v>1</v>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>[1586]</t>
+        </is>
+      </c>
+      <c r="E109" t="n">
+        <v>1586</v>
+      </c>
+      <c r="F109" t="n">
+        <v>2000</v>
+      </c>
+      <c r="G109" t="n">
+        <v>0.793</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>2036</v>
+      </c>
+      <c r="B110" t="n">
+        <v>374999</v>
+      </c>
+      <c r="C110" t="n">
+        <v>1</v>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>[1701]</t>
+        </is>
+      </c>
+      <c r="E110" t="n">
+        <v>1701</v>
+      </c>
+      <c r="F110" t="n">
+        <v>2083</v>
+      </c>
+      <c r="G110" t="n">
+        <v>0.8166</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>2041</v>
+      </c>
+      <c r="B111" t="n">
+        <v>599999</v>
+      </c>
+      <c r="C111" t="n">
+        <v>1</v>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>[1605]</t>
+        </is>
+      </c>
+      <c r="E111" t="n">
+        <v>1605</v>
+      </c>
+      <c r="F111" t="n">
+        <v>1971</v>
+      </c>
+      <c r="G111" t="n">
+        <v>0.8143</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>2045</v>
+      </c>
+      <c r="B112" t="n">
+        <v>449999</v>
+      </c>
+      <c r="C112" t="n">
+        <v>1</v>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>[1638]</t>
+        </is>
+      </c>
+      <c r="E112" t="n">
+        <v>1638</v>
+      </c>
+      <c r="F112" t="n">
+        <v>2028</v>
+      </c>
+      <c r="G112" t="n">
+        <v>0.8077</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>2048</v>
+      </c>
+      <c r="B113" t="n">
+        <v>499999</v>
+      </c>
+      <c r="C113" t="n">
+        <v>1</v>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>[1545]</t>
+        </is>
+      </c>
+      <c r="E113" t="n">
+        <v>1545</v>
+      </c>
+      <c r="F113" t="n">
+        <v>1939</v>
+      </c>
+      <c r="G113" t="n">
+        <v>0.7968</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>2053</v>
+      </c>
+      <c r="B114" t="n">
+        <v>224999</v>
+      </c>
+      <c r="C114" t="n">
+        <v>1</v>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>[1587]</t>
+        </is>
+      </c>
+      <c r="E114" t="n">
+        <v>1587</v>
+      </c>
+      <c r="F114" t="n">
+        <v>1962</v>
+      </c>
+      <c r="G114" t="n">
+        <v>0.8089</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>2057</v>
+      </c>
+      <c r="B115" t="n">
+        <v>349999</v>
+      </c>
+      <c r="C115" t="n">
+        <v>1</v>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>[1612]</t>
+        </is>
+      </c>
+      <c r="E115" t="n">
+        <v>1612</v>
+      </c>
+      <c r="F115" t="n">
+        <v>2013</v>
+      </c>
+      <c r="G115" t="n">
+        <v>0.8008</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>2061</v>
+      </c>
+      <c r="B116" t="n">
+        <v>824999</v>
+      </c>
+      <c r="C116" t="n">
+        <v>1</v>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>[1637]</t>
+        </is>
+      </c>
+      <c r="E116" t="n">
+        <v>1637</v>
+      </c>
+      <c r="F116" t="n">
+        <v>2002</v>
+      </c>
+      <c r="G116" t="n">
+        <v>0.8177</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>2064</v>
+      </c>
+      <c r="B117" t="n">
+        <v>249999</v>
+      </c>
+      <c r="C117" t="n">
+        <v>1</v>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>[1562]</t>
+        </is>
+      </c>
+      <c r="E117" t="n">
+        <v>1562</v>
+      </c>
+      <c r="F117" t="n">
+        <v>1956</v>
+      </c>
+      <c r="G117" t="n">
+        <v>0.7986</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>2068</v>
+      </c>
+      <c r="B118" t="n">
+        <v>424999</v>
+      </c>
+      <c r="C118" t="n">
+        <v>1</v>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>[1532]</t>
+        </is>
+      </c>
+      <c r="E118" t="n">
+        <v>1532</v>
+      </c>
+      <c r="F118" t="n">
+        <v>1941</v>
+      </c>
+      <c r="G118" t="n">
+        <v>0.7893</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>2073</v>
+      </c>
+      <c r="B119" t="n">
+        <v>249999</v>
+      </c>
+      <c r="C119" t="n">
+        <v>1</v>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>[1552]</t>
+        </is>
+      </c>
+      <c r="E119" t="n">
+        <v>1552</v>
+      </c>
+      <c r="F119" t="n">
+        <v>2004</v>
+      </c>
+      <c r="G119" t="n">
+        <v>0.7745</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>2077</v>
+      </c>
+      <c r="B120" t="n">
+        <v>524999</v>
+      </c>
+      <c r="C120" t="n">
+        <v>1</v>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>[1608]</t>
+        </is>
+      </c>
+      <c r="E120" t="n">
+        <v>1608</v>
+      </c>
+      <c r="F120" t="n">
+        <v>2018</v>
+      </c>
+      <c r="G120" t="n">
+        <v>0.7968</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>2081</v>
+      </c>
+      <c r="B121" t="n">
+        <v>374999</v>
+      </c>
+      <c r="C121" t="n">
+        <v>1</v>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>[1643]</t>
+        </is>
+      </c>
+      <c r="E121" t="n">
+        <v>1643</v>
+      </c>
+      <c r="F121" t="n">
+        <v>2037</v>
+      </c>
+      <c r="G121" t="n">
+        <v>0.8066</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>2085</v>
+      </c>
+      <c r="B122" t="n">
+        <v>249999</v>
+      </c>
+      <c r="C122" t="n">
+        <v>1</v>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>[1629]</t>
+        </is>
+      </c>
+      <c r="E122" t="n">
+        <v>1629</v>
+      </c>
+      <c r="F122" t="n">
+        <v>2001</v>
+      </c>
+      <c r="G122" t="n">
+        <v>0.8141</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>2089</v>
+      </c>
+      <c r="B123" t="n">
+        <v>799999</v>
+      </c>
+      <c r="C123" t="n">
+        <v>1</v>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>[1595]</t>
+        </is>
+      </c>
+      <c r="E123" t="n">
+        <v>1595</v>
+      </c>
+      <c r="F123" t="n">
+        <v>1985</v>
+      </c>
+      <c r="G123" t="n">
+        <v>0.8035</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>2093</v>
+      </c>
+      <c r="B124" t="n">
+        <v>399999</v>
+      </c>
+      <c r="C124" t="n">
+        <v>1</v>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>[1572]</t>
+        </is>
+      </c>
+      <c r="E124" t="n">
+        <v>1572</v>
+      </c>
+      <c r="F124" t="n">
+        <v>1959</v>
+      </c>
+      <c r="G124" t="n">
+        <v>0.8025</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>2097</v>
+      </c>
+      <c r="B125" t="n">
+        <v>199999</v>
+      </c>
+      <c r="C125" t="n">
+        <v>1</v>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>[1561]</t>
+        </is>
+      </c>
+      <c r="E125" t="n">
+        <v>1561</v>
+      </c>
+      <c r="F125" t="n">
+        <v>1966</v>
+      </c>
+      <c r="G125" t="n">
+        <v>0.794</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>2101</v>
+      </c>
+      <c r="B126" t="n">
+        <v>549999</v>
+      </c>
+      <c r="C126" t="n">
+        <v>1</v>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>[1625]</t>
+        </is>
+      </c>
+      <c r="E126" t="n">
+        <v>1625</v>
+      </c>
+      <c r="F126" t="n">
+        <v>2024</v>
+      </c>
+      <c r="G126" t="n">
+        <v>0.8028999999999999</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>2105</v>
+      </c>
+      <c r="B127" t="n">
+        <v>524999</v>
+      </c>
+      <c r="C127" t="n">
+        <v>1</v>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>[1621]</t>
+        </is>
+      </c>
+      <c r="E127" t="n">
+        <v>1621</v>
+      </c>
+      <c r="F127" t="n">
+        <v>2019</v>
+      </c>
+      <c r="G127" t="n">
+        <v>0.8028999999999999</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>2109</v>
+      </c>
+      <c r="B128" t="n">
+        <v>674999</v>
+      </c>
+      <c r="C128" t="n">
+        <v>1</v>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>[1667]</t>
+        </is>
+      </c>
+      <c r="E128" t="n">
+        <v>1667</v>
+      </c>
+      <c r="F128" t="n">
+        <v>2007</v>
+      </c>
+      <c r="G128" t="n">
+        <v>0.8306</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>2112</v>
+      </c>
+      <c r="B129" t="n">
+        <v>49999</v>
+      </c>
+      <c r="C129" t="n">
+        <v>1</v>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>[1621]</t>
+        </is>
+      </c>
+      <c r="E129" t="n">
+        <v>1621</v>
+      </c>
+      <c r="F129" t="n">
+        <v>1994</v>
+      </c>
+      <c r="G129" t="n">
+        <v>0.8129</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="n">
+        <v>2116</v>
+      </c>
+      <c r="B130" t="n">
+        <v>174999</v>
+      </c>
+      <c r="C130" t="n">
+        <v>1</v>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>[1626]</t>
+        </is>
+      </c>
+      <c r="E130" t="n">
+        <v>1626</v>
+      </c>
+      <c r="F130" t="n">
+        <v>2006</v>
+      </c>
+      <c r="G130" t="n">
+        <v>0.8106</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="n">
+        <v>2120</v>
+      </c>
+      <c r="B131" t="n">
+        <v>1149999</v>
+      </c>
+      <c r="C131" t="n">
+        <v>1</v>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>[1614]</t>
+        </is>
+      </c>
+      <c r="E131" t="n">
+        <v>1614</v>
+      </c>
+      <c r="F131" t="n">
+        <v>1988</v>
+      </c>
+      <c r="G131" t="n">
+        <v>0.8119</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="n">
+        <v>2124</v>
+      </c>
+      <c r="B132" t="n">
+        <v>524999</v>
+      </c>
+      <c r="C132" t="n">
+        <v>1</v>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>[1618]</t>
+        </is>
+      </c>
+      <c r="E132" t="n">
+        <v>1618</v>
+      </c>
+      <c r="F132" t="n">
+        <v>1998</v>
+      </c>
+      <c r="G132" t="n">
+        <v>0.8098</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="n">
+        <v>2128</v>
+      </c>
+      <c r="B133" t="n">
+        <v>724999</v>
+      </c>
+      <c r="C133" t="n">
+        <v>1</v>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>[1613]</t>
+        </is>
+      </c>
+      <c r="E133" t="n">
+        <v>1613</v>
+      </c>
+      <c r="F133" t="n">
+        <v>1999</v>
+      </c>
+      <c r="G133" t="n">
+        <v>0.8069</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="n">
+        <v>2132</v>
+      </c>
+      <c r="B134" t="n">
+        <v>1024999</v>
+      </c>
+      <c r="C134" t="n">
+        <v>1</v>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>[1682]</t>
+        </is>
+      </c>
+      <c r="E134" t="n">
+        <v>1682</v>
+      </c>
+      <c r="F134" t="n">
+        <v>2070</v>
+      </c>
+      <c r="G134" t="n">
+        <v>0.8126</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="n">
+        <v>2136</v>
+      </c>
+      <c r="B135" t="n">
+        <v>249999</v>
+      </c>
+      <c r="C135" t="n">
+        <v>1</v>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>[1602]</t>
+        </is>
+      </c>
+      <c r="E135" t="n">
+        <v>1602</v>
+      </c>
+      <c r="F135" t="n">
+        <v>1990</v>
+      </c>
+      <c r="G135" t="n">
+        <v>0.805</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="n">
+        <v>2140</v>
+      </c>
+      <c r="B136" t="n">
+        <v>474999</v>
+      </c>
+      <c r="C136" t="n">
+        <v>1</v>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>[1630]</t>
+        </is>
+      </c>
+      <c r="E136" t="n">
+        <v>1630</v>
+      </c>
+      <c r="F136" t="n">
+        <v>1997</v>
+      </c>
+      <c r="G136" t="n">
+        <v>0.8162</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>